<commit_message>
feat: Filter out example rows from Excel templates during upload
</commit_message>
<xml_diff>
--- a/backend/data/templates/clients_template.xlsx
+++ b/backend/data/templates/clients_template.xlsx
@@ -433,11 +433,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="9" customWidth="1" min="1" max="1"/>
     <col width="9" customWidth="1" min="2" max="2"/>
     <col width="4" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="7" customWidth="1" min="5" max="5"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="6" customWidth="1" min="5" max="5"/>
     <col width="8" customWidth="1" min="6" max="6"/>
     <col width="8" customWidth="1" min="7" max="7"/>
     <col width="8" customWidth="1" min="8" max="8"/>
@@ -445,8 +445,8 @@
     <col width="7" customWidth="1" min="10" max="10"/>
     <col width="12" customWidth="1" min="11" max="11"/>
     <col width="6" customWidth="1" min="12" max="12"/>
-    <col width="15" customWidth="1" min="13" max="13"/>
-    <col width="9" customWidth="1" min="14" max="14"/>
+    <col width="14" customWidth="1" min="13" max="13"/>
+    <col width="6" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -524,12 +524,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CUST-0001</t>
+          <t>예시-0001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(주)서울냉동</t>
+          <t>거래처명 예시</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -557,8 +557,16 @@
           <t>17:00</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>Y</t>
@@ -569,7 +577,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>김철수</t>
+          <t>홍길동</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -577,48 +585,32 @@
           <t>02-1234-5678</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>주차공간 협소</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CUST-0002</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>(주)부산물류</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>하차</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>부산광역시 해운대구 센텀동 456</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>3층 A동</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -627,18 +619,10 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>20</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>이영희</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>051-9876-5432</t>
-        </is>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Improve Excel templates with examples and automatic empty row filtering
- Add example rows to all templates (거래처/차량/주문)
- Add 3 empty rows per template for user data entry
- Filter out example rows automatically (예시-, TRUCK-001, ORD- patterns)
- Filter out empty rows automatically (notna check on primary keys)
- Improve user experience: show data entry format without causing upload conflicts
- Templates now include: 1 example row + 3 empty rows
- Parsing logic filters: example rows (예시- prefix) + empty rows (nan primary keys)
- Test results: ✅ 2 user records parsed correctly from test files
</commit_message>
<xml_diff>
--- a/backend/data/templates/clients_template.xlsx
+++ b/backend/data/templates/clients_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <col width="12" customWidth="1" min="11" max="11"/>
     <col width="6" customWidth="1" min="12" max="12"/>
     <col width="14" customWidth="1" min="13" max="13"/>
-    <col width="6" customWidth="1" min="14" max="14"/>
+    <col width="9" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -529,7 +529,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>거래처명 예시</t>
+          <t>(주)서울냉동</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -585,7 +585,11 @@
           <t>02-1234-5678</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>주차공간 협소</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -625,6 +629,82 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>30</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>30</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Complete UVIS transportation management system (#1)
Merging complete UVIS system with temperature auto-fill feature. All 21 phases completed and production tested.
</commit_message>
<xml_diff>
--- a/backend/data/templates/clients_template.xlsx
+++ b/backend/data/templates/clients_template.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="거래처" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="거래처" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>